<commit_message>
6th nov test cases
</commit_message>
<xml_diff>
--- a/LA_Sikuli/src/test/resources/TestData/Test_Data.xlsx
+++ b/LA_Sikuli/src/test/resources/TestData/Test_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\X023840\git\LA_Sikuli\LA_Sikuli\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85297998-34BB-48F5-A827-B6B59EE54D4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC7DB77-43C3-4471-A4CE-4126AC2F1ABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>RunTest</t>
   </si>
@@ -59,26 +59,59 @@
     <t>Class Name</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
     <t>Aim of the script is to Create a Multiple New Stories  and Publish the same</t>
   </si>
   <si>
-    <t>StoryCases</t>
-  </si>
-  <si>
-    <t>VerifyMultipleStoryPublish</t>
+    <t>Aim of the script is to Create a  Multiple New Alerts,Publish and Verify in the GRID</t>
+  </si>
+  <si>
+    <t>FW_UI_0002</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>VerifyPublishScenarios</t>
+  </si>
+  <si>
+    <t>PublishCases</t>
+  </si>
+  <si>
+    <t>Story,TestStoryHeadline,Test,Test,TestMe,Test.V,Test,T,Taslic/,TestStory</t>
+  </si>
+  <si>
+    <t>Aim of the script is to Create Mulitple New  Econs , Publilsh and Verify in the Grid</t>
+  </si>
+  <si>
+    <t>FW_UI_0003</t>
+  </si>
+  <si>
+    <t>Alert,TestAlertHeadline,Test,Test,TestMe,Test.V, Test,T,Taslic/,NA</t>
+  </si>
+  <si>
+    <t>Econ,64424509456,7,5,NA,NA, NA,NA,NA,NA</t>
+  </si>
+  <si>
+    <t>Aim of the script is to Create a New Story and Save as Template</t>
+  </si>
+  <si>
+    <t>TemplateCases</t>
+  </si>
+  <si>
+    <t>FW_UI_0004</t>
+  </si>
+  <si>
+    <t>VerifyTemplateScenarios</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -92,6 +125,11 @@
       <b/>
       <sz val="10"/>
       <color indexed="17"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -110,7 +148,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -133,11 +171,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -149,6 +222,27 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -398,7 +492,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CBB49106-BC95-4A00-9B23-0E30E5D20288}" name="Table2" displayName="Table2" ref="A1:F2" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CBB49106-BC95-4A00-9B23-0E30E5D20288}" name="Table2" displayName="Table2" ref="A1:F5" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{E8C12C75-5AB5-4A43-A3C6-442932DE8960}" name="RunTest" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{2D0C15F7-7463-4837-A664-2CE60CA101D5}" name="TC_ID" dataDxfId="4"/>
@@ -699,10 +793,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -738,23 +832,83 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="4" t="s">
+    </row>
+    <row r="3" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="B3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>9</v>
+      <c r="B5" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Econ data formatting Cases, Cyclic alert default language cases
</commit_message>
<xml_diff>
--- a/LA_Sikuli/src/test/resources/TestData/Test_Data.xlsx
+++ b/LA_Sikuli/src/test/resources/TestData/Test_Data.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\X023840\git\LA_Sikuli\LA_Sikuli\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A20D5FBD-5F9B-4678-AA27-094E35E22440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B30F9B8-F16C-40A0-86B1-FDA68EFEAF86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Test Cases'!#REF!</definedName>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1434" uniqueCount="655">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1822" uniqueCount="803">
   <si>
     <t>RunTest</t>
   </si>
@@ -2004,6 +2005,450 @@
   </si>
   <si>
     <t>Econ,644245094516,1..0,2--0,NA,NA,NA,NA,NA,NA,PublishDisabled</t>
+  </si>
+  <si>
+    <t>Story,TestStoryHeadline1,Test,Test,TestMe,Test.V,Test,T,Taslic/,TestStory,PublishEnabled</t>
+  </si>
+  <si>
+    <t>Alert,TestAlertHeadline1,Test,Test,TestMe,Test.V,Test,T,Taslic/,NA,PublishEnabled</t>
+  </si>
+  <si>
+    <t>VerifyTemplateRecreateScenarios</t>
+  </si>
+  <si>
+    <t>VerifyPackageTemplateRecreateScenarios</t>
+  </si>
+  <si>
+    <t>VerifyCompanyNumberFormatting</t>
+  </si>
+  <si>
+    <t>CompanyDataCases</t>
+  </si>
+  <si>
+    <t>Japanese,NO,NO,SINGLE</t>
+  </si>
+  <si>
+    <t>Japanese,NO,NO,K</t>
+  </si>
+  <si>
+    <t>Japanese,NO,NO,MLN</t>
+  </si>
+  <si>
+    <t>Japanese,NO,NO,BLN</t>
+  </si>
+  <si>
+    <t>Japanese,NO,NO,TRLN</t>
+  </si>
+  <si>
+    <t>English,NO,NO,SINGLE</t>
+  </si>
+  <si>
+    <t>English,NO,NO,K</t>
+  </si>
+  <si>
+    <t>English,NO,NO,MLN</t>
+  </si>
+  <si>
+    <t>English,NO,NO,BLN</t>
+  </si>
+  <si>
+    <t>English,NO,NO,TRLN</t>
+  </si>
+  <si>
+    <t>French,NO,NO,SINGLE</t>
+  </si>
+  <si>
+    <t>French,NO,NO,K</t>
+  </si>
+  <si>
+    <t>French,NO,NO,MLN</t>
+  </si>
+  <si>
+    <t>French,NO,NO,BLN</t>
+  </si>
+  <si>
+    <t>French,NO,NO,TRLN</t>
+  </si>
+  <si>
+    <t>Japanese,YES,YES,K</t>
+  </si>
+  <si>
+    <t>Japanese,YES,YES,MLN</t>
+  </si>
+  <si>
+    <t>Japanese,YES,YES,TRLN</t>
+  </si>
+  <si>
+    <t>Japanese,YES,YES,BLN</t>
+  </si>
+  <si>
+    <t>English,YES,YES,SINGLE</t>
+  </si>
+  <si>
+    <t>English,YES,YES,K</t>
+  </si>
+  <si>
+    <t>English,YES,YES,MLN</t>
+  </si>
+  <si>
+    <t>English,YES,YES,BLN</t>
+  </si>
+  <si>
+    <t>English,YES,YES,TRLN</t>
+  </si>
+  <si>
+    <t>French,YES,YES,SINGLE</t>
+  </si>
+  <si>
+    <t>French,YES,YES,K</t>
+  </si>
+  <si>
+    <t>French,YES,YES,MLN</t>
+  </si>
+  <si>
+    <t>French,YES,YES,BLN</t>
+  </si>
+  <si>
+    <t>French,YES,YES,TRLN</t>
+  </si>
+  <si>
+    <t>Japanese,YES,NO,SINGLE</t>
+  </si>
+  <si>
+    <t>Japanese,YES,NO,K</t>
+  </si>
+  <si>
+    <t>Japanese,YES,NO,MLN</t>
+  </si>
+  <si>
+    <t>Japanese,YES,NO,BLN</t>
+  </si>
+  <si>
+    <t>Japanese,YES,NO,TRLN</t>
+  </si>
+  <si>
+    <t>English,YES,NO,SINGLE</t>
+  </si>
+  <si>
+    <t>English,YES,NO,K</t>
+  </si>
+  <si>
+    <t>English,YES,NO,MLN</t>
+  </si>
+  <si>
+    <t>English,YES,NO,BLN</t>
+  </si>
+  <si>
+    <t>English,YES,NO,TRLN</t>
+  </si>
+  <si>
+    <t>French,YES,NO,SINGLE</t>
+  </si>
+  <si>
+    <t>French,YES,NO,K</t>
+  </si>
+  <si>
+    <t>French,YES,NO,MLN</t>
+  </si>
+  <si>
+    <t>French,YES,NO,BLN</t>
+  </si>
+  <si>
+    <t>French,YES,NO,TRLN</t>
+  </si>
+  <si>
+    <t>Japanese,NO,YES,SINGLE</t>
+  </si>
+  <si>
+    <t>Japanese,NO,YES,K</t>
+  </si>
+  <si>
+    <t>Japanese,NO,YES,MLN</t>
+  </si>
+  <si>
+    <t>Japanese,NO,YES,BLN</t>
+  </si>
+  <si>
+    <t>Japanese,NO,YES,TRLN</t>
+  </si>
+  <si>
+    <t>English,NO,YES,SINGLE</t>
+  </si>
+  <si>
+    <t>English,NO,YES,K</t>
+  </si>
+  <si>
+    <t>English,NO,YES,MLN</t>
+  </si>
+  <si>
+    <t>English,NO,YES,BLN</t>
+  </si>
+  <si>
+    <t>English,NO,YES,TRLN</t>
+  </si>
+  <si>
+    <t>French,NO,YES,SINGLE</t>
+  </si>
+  <si>
+    <t>French,NO,YES,K</t>
+  </si>
+  <si>
+    <t>French,NO,YES,MLN</t>
+  </si>
+  <si>
+    <t>French,NO,YES,BLN</t>
+  </si>
+  <si>
+    <t>French,NO,YES,TRLN</t>
+  </si>
+  <si>
+    <t>DESCR</t>
+  </si>
+  <si>
+    <t>Japanese,YES,YES,SINGLE,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>Japanese,YES,YES,K,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>Japanese,YES,YES,MLN,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>Japanese,YES,YES,BLN,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>Japanese,YES,YES,TRLN,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>English,YES,YES,SINGLE,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>English,YES,YES,K,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>English,YES,YES,MLN,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>English,YES,YES,BLN,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>English,YES,YES,TRLN,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>French,YES,YES,SINGLE,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>French,YES,YES,K,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>French,YES,YES,MLN,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>French,YES,YES,BLN,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>French,YES,YES,TRLN,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>Japanese,NO,NO,SINGLE,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>Japanese,NO,NO,K,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>Japanese,NO,NO,MLN,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>Japanese,NO,NO,BLN,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>Japanese,NO,NO,TRLN,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>English,NO,NO,SINGLE,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>English,NO,NO,K,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>English,NO,NO,MLN,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>English,NO,NO,BLN,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>English,NO,NO,TRLN,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>French,NO,NO,SINGLE,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>French,NO,NO,K,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>French,NO,NO,MLN,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>French,NO,NO,BLN,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>French,NO,NO,TRLN,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>Japanese,YES,NO,SINGLE,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>Japanese,YES,NO,K,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>Japanese,YES,NO,MLN,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>Japanese,YES,NO,BLN,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>Japanese,YES,NO,TRLN,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>English,YES,NO,SINGLE,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>English,YES,NO,K,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>English,YES,NO,MLN,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>English,YES,NO,BLN,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>English,YES,NO,TRLN,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>French,YES,NO,SINGLE,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>French,YES,NO,K,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>French,YES,NO,MLN,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>French,YES,NO,BLN,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>French,YES,NO,TRLN,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>Japanese,NO,YES,SINGLE,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>Japanese,NO,YES,K,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>Japanese,NO,YES,MLN,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>Japanese,NO,YES,BLN,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>Japanese,NO,YES,TRLN,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>English,NO,YES,SINGLE,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>English,NO,YES,K,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>English,NO,YES,MLN,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>English,NO,YES,BLN,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>English,NO,YES,TRLN,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>French,NO,YES,SINGLE,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>French,NO,YES,K,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>French,NO,YES,MLN,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>French,NO,YES,BLN,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>French,NO,YES,TRLN,DESCR,1234567,2.0,3.8897</t>
+  </si>
+  <si>
+    <t>EconDataCases</t>
+  </si>
+  <si>
+    <t>VerifyEconDataFormatting</t>
+  </si>
+  <si>
+    <t>English,NO,YES,64424509450,4.567,+2.1</t>
+  </si>
+  <si>
+    <t>French,NO,YES,64424509450,4.567,+2.1</t>
+  </si>
+  <si>
+    <t>Japanese,NO,YES,64424509450,4.567,+2.1</t>
+  </si>
+  <si>
+    <t>Aim of the script is to Verify Auto Round Econ Data for Chinese Language with ARE - FALSE and LNF - FALSE</t>
+  </si>
+  <si>
+    <t>Aim of the script is to Verify Auto Round Econ Data for Chinese Language with ARE - FALSE and LNF - TRUE</t>
+  </si>
+  <si>
+    <t>Chinese,NO,YES,64424509450,4.567,+2.1</t>
+  </si>
+  <si>
+    <t>English,YES,YES,64424509450,4.567,+2.1</t>
+  </si>
+  <si>
+    <t>French,YES,YES,64424509450,4.567,+2.1</t>
+  </si>
+  <si>
+    <t>Japanese,YES,YES,64424509450,4.567,+2.1</t>
+  </si>
+  <si>
+    <t>Chinese,YES,YES,64424509450,4.567,+2.1</t>
+  </si>
+  <si>
+    <t>English,NO,NO,64424509450,4.567,+2.1</t>
+  </si>
+  <si>
+    <t>French,NO,NO,64424509450,4.567,+2.1</t>
+  </si>
+  <si>
+    <t>Japanese,NO,NO,64424509450,4.567,+2.1</t>
+  </si>
+  <si>
+    <t>Chinese,NO,NO,64424509450,4.567,+2.1</t>
+  </si>
+  <si>
+    <t>English,YES,NO,64424509450,4.567,+2.1</t>
+  </si>
+  <si>
+    <t>French,YES,NO,64424509450,4.567,+2.1</t>
+  </si>
+  <si>
+    <t>Japanese,YES,NO,64424509450,4.567,+2.1</t>
+  </si>
+  <si>
+    <t>Chinese,YES,NO,64424509450,4.567,+2.1</t>
+  </si>
+  <si>
+    <t>VerifyCyclicAlertLanguage</t>
+  </si>
+  <si>
+    <t>Chinese,TESTALERTHEADLINECyclical,TEST,TEST,TESTME,TEST.V,TEST</t>
   </si>
 </sst>
 </file>
@@ -2038,7 +2483,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2048,6 +2493,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2140,7 +2597,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -2177,6 +2634,33 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2728,8 +3212,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F284"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A143" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D97" sqref="D97"/>
+    <sheetView tabSelected="1" topLeftCell="A141" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A164" sqref="A164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2739,8 +3223,8 @@
     <col min="3" max="3" width="31.28515625" style="3" customWidth="1"/>
     <col min="4" max="4" width="40.140625" style="3" customWidth="1"/>
     <col min="5" max="5" width="20.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="162.5703125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="109" style="2" customWidth="1"/>
+    <col min="6" max="6" width="106.5703125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" style="2" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -4885,682 +5369,682 @@
       </c>
     </row>
     <row r="108" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="4" t="s">
-        <v>621</v>
-      </c>
-      <c r="B108" s="4" t="s">
+      <c r="A108" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="B108" s="15" t="s">
         <v>429</v>
       </c>
-      <c r="C108" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="D108" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="E108" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="F108" s="11" t="s">
+      <c r="C108" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="D108" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="E108" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="F108" s="14" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="109" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="4" t="s">
-        <v>621</v>
-      </c>
-      <c r="B109" s="4" t="s">
+      <c r="A109" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="B109" s="15" t="s">
         <v>430</v>
       </c>
-      <c r="C109" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="D109" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="E109" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="F109" s="11" t="s">
+      <c r="C109" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="D109" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="E109" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="F109" s="14" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="110" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="4" t="s">
-        <v>621</v>
-      </c>
-      <c r="B110" s="4" t="s">
+      <c r="A110" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="B110" s="15" t="s">
         <v>431</v>
       </c>
-      <c r="C110" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="D110" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="E110" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="F110" s="11" t="s">
+      <c r="C110" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="D110" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="E110" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="F110" s="14" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="111" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="4" t="s">
-        <v>621</v>
-      </c>
-      <c r="B111" s="4" t="s">
+      <c r="A111" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="B111" s="15" t="s">
         <v>432</v>
       </c>
-      <c r="C111" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="D111" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="E111" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="F111" s="11" t="s">
+      <c r="C111" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="D111" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="E111" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="F111" s="14" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="112" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="4" t="s">
-        <v>621</v>
-      </c>
-      <c r="B112" s="4" t="s">
+      <c r="A112" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="B112" s="15" t="s">
         <v>433</v>
       </c>
-      <c r="C112" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="D112" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="E112" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="F112" s="11" t="s">
+      <c r="C112" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="D112" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="E112" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="F112" s="14" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="113" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="4" t="s">
-        <v>621</v>
-      </c>
-      <c r="B113" s="4" t="s">
+      <c r="A113" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="B113" s="15" t="s">
         <v>434</v>
       </c>
-      <c r="C113" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="D113" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="E113" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="F113" s="11" t="s">
+      <c r="C113" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="D113" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="E113" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="F113" s="14" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="114" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="4" t="s">
-        <v>621</v>
-      </c>
-      <c r="B114" s="4" t="s">
+      <c r="A114" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="B114" s="15" t="s">
         <v>435</v>
       </c>
-      <c r="C114" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="D114" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="E114" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="F114" s="11" t="s">
+      <c r="C114" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="D114" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="E114" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="F114" s="14" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="115" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="4" t="s">
-        <v>621</v>
-      </c>
-      <c r="B115" s="4" t="s">
+      <c r="A115" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="B115" s="15" t="s">
         <v>436</v>
       </c>
-      <c r="C115" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="D115" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="E115" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="F115" s="11" t="s">
+      <c r="C115" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="D115" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="E115" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="F115" s="14" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="116" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="4" t="s">
-        <v>621</v>
-      </c>
-      <c r="B116" s="4" t="s">
+      <c r="A116" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="B116" s="15" t="s">
         <v>437</v>
       </c>
-      <c r="C116" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="D116" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="E116" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="F116" s="11" t="s">
+      <c r="C116" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="D116" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="E116" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="F116" s="14" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="117" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="4" t="s">
-        <v>621</v>
-      </c>
-      <c r="B117" s="4" t="s">
+      <c r="A117" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="B117" s="15" t="s">
         <v>438</v>
       </c>
-      <c r="C117" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="D117" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="E117" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="F117" s="11" t="s">
+      <c r="C117" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="D117" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="E117" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="F117" s="14" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="118" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="4" t="s">
-        <v>621</v>
-      </c>
-      <c r="B118" s="4" t="s">
+      <c r="A118" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="B118" s="15" t="s">
         <v>439</v>
       </c>
-      <c r="C118" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="D118" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="E118" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="F118" s="11" t="s">
+      <c r="C118" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="D118" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="E118" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="F118" s="14" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="119" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="4" t="s">
-        <v>621</v>
-      </c>
-      <c r="B119" s="4" t="s">
+      <c r="A119" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="B119" s="15" t="s">
         <v>440</v>
       </c>
-      <c r="C119" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="D119" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="E119" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="F119" s="11" t="s">
+      <c r="C119" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="D119" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="E119" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="F119" s="14" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="120" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="4" t="s">
-        <v>621</v>
-      </c>
-      <c r="B120" s="4" t="s">
+      <c r="A120" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="B120" s="15" t="s">
         <v>441</v>
       </c>
-      <c r="C120" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="D120" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="E120" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="F120" s="11" t="s">
+      <c r="C120" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="D120" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="E120" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="F120" s="14" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="121" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="4" t="s">
-        <v>621</v>
-      </c>
-      <c r="B121" s="4" t="s">
+      <c r="A121" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="B121" s="15" t="s">
         <v>442</v>
       </c>
-      <c r="C121" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="D121" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="E121" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="F121" s="11" t="s">
+      <c r="C121" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="D121" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="E121" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="F121" s="14" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="122" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="4" t="s">
-        <v>621</v>
-      </c>
-      <c r="B122" s="4" t="s">
+      <c r="A122" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="B122" s="15" t="s">
         <v>443</v>
       </c>
-      <c r="C122" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="D122" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="E122" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="F122" s="11" t="s">
+      <c r="C122" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="D122" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="E122" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="F122" s="14" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="123" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="4" t="s">
-        <v>621</v>
-      </c>
-      <c r="B123" s="4" t="s">
+      <c r="A123" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="B123" s="15" t="s">
         <v>444</v>
       </c>
-      <c r="C123" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="D123" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="E123" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="F123" s="11" t="s">
+      <c r="C123" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="D123" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="E123" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="F123" s="14" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="124" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="4" t="s">
-        <v>621</v>
-      </c>
-      <c r="B124" s="4" t="s">
+      <c r="A124" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="B124" s="15" t="s">
         <v>445</v>
       </c>
-      <c r="C124" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="D124" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="E124" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="F124" s="11" t="s">
+      <c r="C124" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="D124" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="E124" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="F124" s="14" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="125" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="4" t="s">
-        <v>621</v>
-      </c>
-      <c r="B125" s="4" t="s">
+      <c r="A125" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="B125" s="15" t="s">
         <v>446</v>
       </c>
-      <c r="C125" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="D125" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="E125" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="F125" s="11" t="s">
+      <c r="C125" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="D125" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="E125" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="F125" s="14" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="126" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="4" t="s">
-        <v>621</v>
-      </c>
-      <c r="B126" s="4" t="s">
+      <c r="A126" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="B126" s="15" t="s">
         <v>447</v>
       </c>
-      <c r="C126" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="D126" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="E126" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="F126" s="11" t="s">
+      <c r="C126" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="D126" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="E126" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="F126" s="14" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="127" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="4" t="s">
-        <v>621</v>
-      </c>
-      <c r="B127" s="4" t="s">
+      <c r="A127" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="B127" s="15" t="s">
         <v>448</v>
       </c>
-      <c r="C127" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="D127" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="E127" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="F127" s="11" t="s">
+      <c r="C127" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="D127" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="E127" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="F127" s="14" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="128" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A128" s="4" t="s">
-        <v>621</v>
-      </c>
-      <c r="B128" s="4" t="s">
+      <c r="A128" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="B128" s="15" t="s">
         <v>449</v>
       </c>
-      <c r="C128" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="D128" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="E128" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="F128" s="11" t="s">
+      <c r="C128" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="D128" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="E128" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="F128" s="14" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="129" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A129" s="4" t="s">
-        <v>621</v>
-      </c>
-      <c r="B129" s="4" t="s">
+      <c r="A129" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="B129" s="15" t="s">
         <v>450</v>
       </c>
-      <c r="C129" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="D129" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="E129" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="F129" s="11" t="s">
+      <c r="C129" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="D129" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="E129" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="F129" s="14" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="130" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A130" s="4" t="s">
-        <v>621</v>
-      </c>
-      <c r="B130" s="4" t="s">
+      <c r="A130" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="B130" s="15" t="s">
         <v>451</v>
       </c>
-      <c r="C130" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="D130" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="E130" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="F130" s="11" t="s">
+      <c r="C130" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="D130" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="E130" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="F130" s="14" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="131" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A131" s="4" t="s">
-        <v>621</v>
-      </c>
-      <c r="B131" s="4" t="s">
+      <c r="A131" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="B131" s="15" t="s">
         <v>452</v>
       </c>
-      <c r="C131" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="D131" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="E131" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="F131" s="11" t="s">
+      <c r="C131" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="D131" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="E131" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="F131" s="14" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="132" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A132" s="4" t="s">
-        <v>621</v>
-      </c>
-      <c r="B132" s="4" t="s">
+      <c r="A132" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="B132" s="15" t="s">
         <v>453</v>
       </c>
-      <c r="C132" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="D132" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="E132" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="F132" s="11" t="s">
+      <c r="C132" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="D132" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="E132" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="F132" s="14" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="133" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A133" s="4" t="s">
-        <v>621</v>
-      </c>
-      <c r="B133" s="4" t="s">
+      <c r="A133" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="B133" s="15" t="s">
         <v>454</v>
       </c>
-      <c r="C133" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="D133" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="E133" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="F133" s="11" t="s">
+      <c r="C133" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="D133" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="E133" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="F133" s="14" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="134" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A134" s="4" t="s">
-        <v>621</v>
-      </c>
-      <c r="B134" s="4" t="s">
+      <c r="A134" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="B134" s="15" t="s">
         <v>455</v>
       </c>
-      <c r="C134" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="D134" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="E134" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="F134" s="11" t="s">
+      <c r="C134" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="D134" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="E134" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="F134" s="14" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="135" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A135" s="4" t="s">
-        <v>621</v>
-      </c>
-      <c r="B135" s="4" t="s">
+      <c r="A135" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="B135" s="15" t="s">
         <v>456</v>
       </c>
-      <c r="C135" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="D135" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="E135" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="F135" s="11" t="s">
+      <c r="C135" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="D135" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="E135" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="F135" s="14" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="136" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A136" s="4" t="s">
-        <v>621</v>
-      </c>
-      <c r="B136" s="4" t="s">
+      <c r="A136" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="B136" s="15" t="s">
         <v>457</v>
       </c>
-      <c r="C136" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="D136" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="E136" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="F136" s="11" t="s">
+      <c r="C136" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="D136" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="E136" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="F136" s="14" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="137" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A137" s="4" t="s">
-        <v>621</v>
-      </c>
-      <c r="B137" s="4" t="s">
+      <c r="A137" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="B137" s="15" t="s">
         <v>458</v>
       </c>
-      <c r="C137" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="D137" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="E137" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="F137" s="11" t="s">
+      <c r="C137" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="D137" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="E137" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="F137" s="14" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="138" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A138" s="4" t="s">
-        <v>621</v>
-      </c>
-      <c r="B138" s="4" t="s">
+      <c r="A138" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="B138" s="15" t="s">
         <v>459</v>
       </c>
-      <c r="C138" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="D138" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="E138" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="F138" s="11" t="s">
+      <c r="C138" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="D138" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="E138" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="F138" s="14" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="139" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A139" s="4" t="s">
-        <v>621</v>
-      </c>
-      <c r="B139" s="4" t="s">
+      <c r="A139" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="B139" s="15" t="s">
         <v>460</v>
       </c>
-      <c r="C139" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="D139" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="E139" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="F139" s="11" t="s">
+      <c r="C139" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="D139" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="E139" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="F139" s="14" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="140" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A140" s="4" t="s">
-        <v>621</v>
-      </c>
-      <c r="B140" s="4" t="s">
+      <c r="A140" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="B140" s="15" t="s">
         <v>461</v>
       </c>
-      <c r="C140" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="D140" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="E140" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="F140" s="11" t="s">
+      <c r="C140" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="D140" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="E140" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="F140" s="14" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="141" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A141" s="4" t="s">
-        <v>621</v>
-      </c>
-      <c r="B141" s="4" t="s">
+      <c r="A141" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="B141" s="15" t="s">
         <v>462</v>
       </c>
-      <c r="C141" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="D141" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="E141" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="F141" s="11" t="s">
+      <c r="C141" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="D141" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="E141" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="F141" s="14" t="s">
         <v>210</v>
       </c>
     </row>
@@ -5771,9 +6255,15 @@
       <c r="B152" s="4" t="s">
         <v>473</v>
       </c>
-      <c r="C152" s="9"/>
-      <c r="D152" s="4"/>
-      <c r="E152" s="10"/>
+      <c r="C152" s="9" t="s">
+        <v>657</v>
+      </c>
+      <c r="D152" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E152" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="F152" s="11" t="s">
         <v>221</v>
       </c>
@@ -5785,9 +6275,15 @@
       <c r="B153" s="4" t="s">
         <v>474</v>
       </c>
-      <c r="C153" s="9"/>
-      <c r="D153" s="4"/>
-      <c r="E153" s="10"/>
+      <c r="C153" s="9" t="s">
+        <v>657</v>
+      </c>
+      <c r="D153" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E153" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="F153" s="11" t="s">
         <v>222</v>
       </c>
@@ -5799,9 +6295,15 @@
       <c r="B154" s="4" t="s">
         <v>475</v>
       </c>
-      <c r="C154" s="9"/>
-      <c r="D154" s="4"/>
-      <c r="E154" s="10"/>
+      <c r="C154" s="9" t="s">
+        <v>657</v>
+      </c>
+      <c r="D154" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E154" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="F154" s="11" t="s">
         <v>223</v>
       </c>
@@ -5813,9 +6315,15 @@
       <c r="B155" s="4" t="s">
         <v>476</v>
       </c>
-      <c r="C155" s="9"/>
-      <c r="D155" s="4"/>
-      <c r="E155" s="10"/>
+      <c r="C155" s="8" t="s">
+        <v>658</v>
+      </c>
+      <c r="D155" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E155" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="F155" s="11" t="s">
         <v>224</v>
       </c>
@@ -5827,9 +6335,15 @@
       <c r="B156" s="4" t="s">
         <v>477</v>
       </c>
-      <c r="C156" s="9"/>
-      <c r="D156" s="4"/>
-      <c r="E156" s="10"/>
+      <c r="C156" s="8" t="s">
+        <v>658</v>
+      </c>
+      <c r="D156" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E156" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="F156" s="11" t="s">
         <v>225</v>
       </c>
@@ -5841,9 +6355,15 @@
       <c r="B157" s="4" t="s">
         <v>478</v>
       </c>
-      <c r="C157" s="9"/>
-      <c r="D157" s="4"/>
-      <c r="E157" s="10"/>
+      <c r="C157" s="8" t="s">
+        <v>658</v>
+      </c>
+      <c r="D157" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E157" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="F157" s="11" t="s">
         <v>226</v>
       </c>
@@ -5855,9 +6375,15 @@
       <c r="B158" s="4" t="s">
         <v>479</v>
       </c>
-      <c r="C158" s="9"/>
-      <c r="D158" s="4"/>
-      <c r="E158" s="10"/>
+      <c r="C158" s="8" t="s">
+        <v>658</v>
+      </c>
+      <c r="D158" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E158" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="F158" s="11" t="s">
         <v>227</v>
       </c>
@@ -5869,9 +6395,15 @@
       <c r="B159" s="4" t="s">
         <v>480</v>
       </c>
-      <c r="C159" s="9"/>
-      <c r="D159" s="4"/>
-      <c r="E159" s="10"/>
+      <c r="C159" s="8" t="s">
+        <v>658</v>
+      </c>
+      <c r="D159" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E159" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="F159" s="11" t="s">
         <v>228</v>
       </c>
@@ -5883,9 +6415,15 @@
       <c r="B160" s="4" t="s">
         <v>481</v>
       </c>
-      <c r="C160" s="9"/>
-      <c r="D160" s="4"/>
-      <c r="E160" s="10"/>
+      <c r="C160" s="8" t="s">
+        <v>658</v>
+      </c>
+      <c r="D160" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E160" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="F160" s="11" t="s">
         <v>229</v>
       </c>
@@ -5897,9 +6435,15 @@
       <c r="B161" s="4" t="s">
         <v>482</v>
       </c>
-      <c r="C161" s="9"/>
-      <c r="D161" s="4"/>
-      <c r="E161" s="10"/>
+      <c r="C161" s="8" t="s">
+        <v>658</v>
+      </c>
+      <c r="D161" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E161" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="F161" s="11" t="s">
         <v>229</v>
       </c>
@@ -5911,9 +6455,15 @@
       <c r="B162" s="4" t="s">
         <v>483</v>
       </c>
-      <c r="C162" s="9"/>
-      <c r="D162" s="4"/>
-      <c r="E162" s="10"/>
+      <c r="C162" s="8" t="s">
+        <v>635</v>
+      </c>
+      <c r="D162" s="5" t="s">
+        <v>656</v>
+      </c>
+      <c r="E162" s="6" t="s">
+        <v>72</v>
+      </c>
       <c r="F162" s="11" t="s">
         <v>230</v>
       </c>
@@ -5925,24 +6475,36 @@
       <c r="B163" s="4" t="s">
         <v>484</v>
       </c>
-      <c r="C163" s="9"/>
-      <c r="D163" s="4"/>
-      <c r="E163" s="10"/>
+      <c r="C163" s="8" t="s">
+        <v>635</v>
+      </c>
+      <c r="D163" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="E163" s="6" t="s">
+        <v>72</v>
+      </c>
       <c r="F163" s="11" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="164" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A164" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B164" s="4" t="s">
+    <row r="164" spans="1:6" s="21" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A164" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B164" s="17" t="s">
         <v>485</v>
       </c>
-      <c r="C164" s="9"/>
-      <c r="D164" s="4"/>
-      <c r="E164" s="10"/>
-      <c r="F164" s="11" t="s">
+      <c r="C164" s="18" t="s">
+        <v>801</v>
+      </c>
+      <c r="D164" s="17" t="s">
+        <v>802</v>
+      </c>
+      <c r="E164" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F164" s="20" t="s">
         <v>232</v>
       </c>
     </row>
@@ -6413,9 +6975,15 @@
       <c r="B188" s="4" t="s">
         <v>509</v>
       </c>
-      <c r="C188" s="9"/>
-      <c r="D188" s="4"/>
-      <c r="E188" s="10"/>
+      <c r="C188" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D188" s="4" t="s">
+        <v>721</v>
+      </c>
+      <c r="E188" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F188" s="11" t="s">
         <v>249</v>
       </c>
@@ -6427,9 +6995,15 @@
       <c r="B189" s="4" t="s">
         <v>510</v>
       </c>
-      <c r="C189" s="9"/>
-      <c r="D189" s="4"/>
-      <c r="E189" s="10"/>
+      <c r="C189" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D189" s="4" t="s">
+        <v>722</v>
+      </c>
+      <c r="E189" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F189" s="11" t="s">
         <v>250</v>
       </c>
@@ -6441,9 +7015,15 @@
       <c r="B190" s="4" t="s">
         <v>511</v>
       </c>
-      <c r="C190" s="9"/>
-      <c r="D190" s="4"/>
-      <c r="E190" s="10"/>
+      <c r="C190" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D190" s="4" t="s">
+        <v>723</v>
+      </c>
+      <c r="E190" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F190" s="11" t="s">
         <v>251</v>
       </c>
@@ -6455,9 +7035,15 @@
       <c r="B191" s="4" t="s">
         <v>512</v>
       </c>
-      <c r="C191" s="9"/>
-      <c r="D191" s="4"/>
-      <c r="E191" s="10"/>
+      <c r="C191" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D191" s="4" t="s">
+        <v>724</v>
+      </c>
+      <c r="E191" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F191" s="11" t="s">
         <v>252</v>
       </c>
@@ -6469,9 +7055,15 @@
       <c r="B192" s="4" t="s">
         <v>513</v>
       </c>
-      <c r="C192" s="9"/>
-      <c r="D192" s="4"/>
-      <c r="E192" s="10"/>
+      <c r="C192" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D192" s="4" t="s">
+        <v>725</v>
+      </c>
+      <c r="E192" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F192" s="11" t="s">
         <v>253</v>
       </c>
@@ -6483,9 +7075,15 @@
       <c r="B193" s="4" t="s">
         <v>514</v>
       </c>
-      <c r="C193" s="9"/>
-      <c r="D193" s="4"/>
-      <c r="E193" s="10"/>
+      <c r="C193" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D193" s="4" t="s">
+        <v>726</v>
+      </c>
+      <c r="E193" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F193" s="11" t="s">
         <v>254</v>
       </c>
@@ -6497,9 +7095,15 @@
       <c r="B194" s="4" t="s">
         <v>515</v>
       </c>
-      <c r="C194" s="9"/>
-      <c r="D194" s="4"/>
-      <c r="E194" s="10"/>
+      <c r="C194" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D194" s="4" t="s">
+        <v>727</v>
+      </c>
+      <c r="E194" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F194" s="11" t="s">
         <v>255</v>
       </c>
@@ -6511,9 +7115,15 @@
       <c r="B195" s="4" t="s">
         <v>516</v>
       </c>
-      <c r="C195" s="9"/>
-      <c r="D195" s="4"/>
-      <c r="E195" s="10"/>
+      <c r="C195" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D195" s="4" t="s">
+        <v>728</v>
+      </c>
+      <c r="E195" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F195" s="11" t="s">
         <v>256</v>
       </c>
@@ -6525,9 +7135,15 @@
       <c r="B196" s="4" t="s">
         <v>517</v>
       </c>
-      <c r="C196" s="9"/>
-      <c r="D196" s="4"/>
-      <c r="E196" s="10"/>
+      <c r="C196" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D196" s="4" t="s">
+        <v>729</v>
+      </c>
+      <c r="E196" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F196" s="11" t="s">
         <v>257</v>
       </c>
@@ -6539,9 +7155,15 @@
       <c r="B197" s="4" t="s">
         <v>518</v>
       </c>
-      <c r="C197" s="9"/>
-      <c r="D197" s="4"/>
-      <c r="E197" s="10"/>
+      <c r="C197" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D197" s="4" t="s">
+        <v>730</v>
+      </c>
+      <c r="E197" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F197" s="11" t="s">
         <v>258</v>
       </c>
@@ -6553,9 +7175,15 @@
       <c r="B198" s="4" t="s">
         <v>519</v>
       </c>
-      <c r="C198" s="9"/>
-      <c r="D198" s="4"/>
-      <c r="E198" s="10"/>
+      <c r="C198" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D198" s="4" t="s">
+        <v>731</v>
+      </c>
+      <c r="E198" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F198" s="11" t="s">
         <v>259</v>
       </c>
@@ -6567,9 +7195,15 @@
       <c r="B199" s="4" t="s">
         <v>520</v>
       </c>
-      <c r="C199" s="9"/>
-      <c r="D199" s="4"/>
-      <c r="E199" s="10"/>
+      <c r="C199" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D199" s="4" t="s">
+        <v>732</v>
+      </c>
+      <c r="E199" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F199" s="11" t="s">
         <v>260</v>
       </c>
@@ -6581,9 +7215,15 @@
       <c r="B200" s="4" t="s">
         <v>521</v>
       </c>
-      <c r="C200" s="9"/>
-      <c r="D200" s="4"/>
-      <c r="E200" s="10"/>
+      <c r="C200" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D200" s="4" t="s">
+        <v>733</v>
+      </c>
+      <c r="E200" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F200" s="11" t="s">
         <v>261</v>
       </c>
@@ -6595,9 +7235,15 @@
       <c r="B201" s="4" t="s">
         <v>522</v>
       </c>
-      <c r="C201" s="9"/>
-      <c r="D201" s="4"/>
-      <c r="E201" s="10"/>
+      <c r="C201" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D201" s="4" t="s">
+        <v>734</v>
+      </c>
+      <c r="E201" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F201" s="11" t="s">
         <v>262</v>
       </c>
@@ -6609,9 +7255,15 @@
       <c r="B202" s="4" t="s">
         <v>523</v>
       </c>
-      <c r="C202" s="9"/>
-      <c r="D202" s="4"/>
-      <c r="E202" s="10"/>
+      <c r="C202" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D202" s="4" t="s">
+        <v>735</v>
+      </c>
+      <c r="E202" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F202" s="11" t="s">
         <v>263</v>
       </c>
@@ -6623,9 +7275,15 @@
       <c r="B203" s="4" t="s">
         <v>524</v>
       </c>
-      <c r="C203" s="9"/>
-      <c r="D203" s="4"/>
-      <c r="E203" s="10"/>
+      <c r="C203" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D203" s="4" t="s">
+        <v>736</v>
+      </c>
+      <c r="E203" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F203" s="11" t="s">
         <v>264</v>
       </c>
@@ -6637,9 +7295,15 @@
       <c r="B204" s="4" t="s">
         <v>525</v>
       </c>
-      <c r="C204" s="9"/>
-      <c r="D204" s="4"/>
-      <c r="E204" s="10"/>
+      <c r="C204" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D204" s="4" t="s">
+        <v>737</v>
+      </c>
+      <c r="E204" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F204" s="11" t="s">
         <v>265</v>
       </c>
@@ -6651,9 +7315,15 @@
       <c r="B205" s="4" t="s">
         <v>526</v>
       </c>
-      <c r="C205" s="9"/>
-      <c r="D205" s="4"/>
-      <c r="E205" s="10"/>
+      <c r="C205" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D205" s="4" t="s">
+        <v>738</v>
+      </c>
+      <c r="E205" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F205" s="11" t="s">
         <v>266</v>
       </c>
@@ -6665,9 +7335,15 @@
       <c r="B206" s="4" t="s">
         <v>527</v>
       </c>
-      <c r="C206" s="9"/>
-      <c r="D206" s="4"/>
-      <c r="E206" s="10"/>
+      <c r="C206" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D206" s="4" t="s">
+        <v>739</v>
+      </c>
+      <c r="E206" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F206" s="11" t="s">
         <v>267</v>
       </c>
@@ -6679,9 +7355,15 @@
       <c r="B207" s="4" t="s">
         <v>528</v>
       </c>
-      <c r="C207" s="9"/>
-      <c r="D207" s="4"/>
-      <c r="E207" s="10"/>
+      <c r="C207" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D207" s="4" t="s">
+        <v>740</v>
+      </c>
+      <c r="E207" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F207" s="11" t="s">
         <v>268</v>
       </c>
@@ -6693,9 +7375,15 @@
       <c r="B208" s="4" t="s">
         <v>529</v>
       </c>
-      <c r="C208" s="9"/>
-      <c r="D208" s="4"/>
-      <c r="E208" s="10"/>
+      <c r="C208" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D208" s="4" t="s">
+        <v>741</v>
+      </c>
+      <c r="E208" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F208" s="11" t="s">
         <v>269</v>
       </c>
@@ -6707,9 +7395,15 @@
       <c r="B209" s="4" t="s">
         <v>530</v>
       </c>
-      <c r="C209" s="9"/>
-      <c r="D209" s="4"/>
-      <c r="E209" s="10"/>
+      <c r="C209" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D209" s="4" t="s">
+        <v>742</v>
+      </c>
+      <c r="E209" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F209" s="11" t="s">
         <v>270</v>
       </c>
@@ -6721,9 +7415,15 @@
       <c r="B210" s="4" t="s">
         <v>531</v>
       </c>
-      <c r="C210" s="9"/>
-      <c r="D210" s="4"/>
-      <c r="E210" s="10"/>
+      <c r="C210" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D210" s="4" t="s">
+        <v>743</v>
+      </c>
+      <c r="E210" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F210" s="11" t="s">
         <v>271</v>
       </c>
@@ -6735,9 +7435,15 @@
       <c r="B211" s="4" t="s">
         <v>532</v>
       </c>
-      <c r="C211" s="9"/>
-      <c r="D211" s="4"/>
-      <c r="E211" s="10"/>
+      <c r="C211" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D211" s="4" t="s">
+        <v>744</v>
+      </c>
+      <c r="E211" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F211" s="11" t="s">
         <v>272</v>
       </c>
@@ -6749,9 +7455,15 @@
       <c r="B212" s="4" t="s">
         <v>533</v>
       </c>
-      <c r="C212" s="9"/>
-      <c r="D212" s="4"/>
-      <c r="E212" s="10"/>
+      <c r="C212" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D212" s="4" t="s">
+        <v>745</v>
+      </c>
+      <c r="E212" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F212" s="11" t="s">
         <v>273</v>
       </c>
@@ -6763,9 +7475,15 @@
       <c r="B213" s="4" t="s">
         <v>534</v>
       </c>
-      <c r="C213" s="9"/>
-      <c r="D213" s="4"/>
-      <c r="E213" s="10"/>
+      <c r="C213" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D213" s="4" t="s">
+        <v>746</v>
+      </c>
+      <c r="E213" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F213" s="11" t="s">
         <v>274</v>
       </c>
@@ -6777,9 +7495,15 @@
       <c r="B214" s="4" t="s">
         <v>535</v>
       </c>
-      <c r="C214" s="9"/>
-      <c r="D214" s="4"/>
-      <c r="E214" s="10"/>
+      <c r="C214" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D214" s="4" t="s">
+        <v>747</v>
+      </c>
+      <c r="E214" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F214" s="11" t="s">
         <v>275</v>
       </c>
@@ -6791,9 +7515,15 @@
       <c r="B215" s="4" t="s">
         <v>536</v>
       </c>
-      <c r="C215" s="9"/>
-      <c r="D215" s="4"/>
-      <c r="E215" s="10"/>
+      <c r="C215" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D215" s="4" t="s">
+        <v>748</v>
+      </c>
+      <c r="E215" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F215" s="11" t="s">
         <v>276</v>
       </c>
@@ -6805,9 +7535,15 @@
       <c r="B216" s="4" t="s">
         <v>537</v>
       </c>
-      <c r="C216" s="9"/>
-      <c r="D216" s="4"/>
-      <c r="E216" s="10"/>
+      <c r="C216" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D216" s="4" t="s">
+        <v>749</v>
+      </c>
+      <c r="E216" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F216" s="11" t="s">
         <v>277</v>
       </c>
@@ -6819,9 +7555,15 @@
       <c r="B217" s="4" t="s">
         <v>538</v>
       </c>
-      <c r="C217" s="9"/>
-      <c r="D217" s="4"/>
-      <c r="E217" s="10"/>
+      <c r="C217" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D217" s="4" t="s">
+        <v>750</v>
+      </c>
+      <c r="E217" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F217" s="11" t="s">
         <v>278</v>
       </c>
@@ -6833,9 +7575,15 @@
       <c r="B218" s="4" t="s">
         <v>539</v>
       </c>
-      <c r="C218" s="9"/>
-      <c r="D218" s="4"/>
-      <c r="E218" s="10"/>
+      <c r="C218" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D218" s="4" t="s">
+        <v>751</v>
+      </c>
+      <c r="E218" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F218" s="11" t="s">
         <v>279</v>
       </c>
@@ -6847,9 +7595,15 @@
       <c r="B219" s="4" t="s">
         <v>540</v>
       </c>
-      <c r="C219" s="9"/>
-      <c r="D219" s="4"/>
-      <c r="E219" s="10"/>
+      <c r="C219" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D219" s="4" t="s">
+        <v>752</v>
+      </c>
+      <c r="E219" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F219" s="11" t="s">
         <v>280</v>
       </c>
@@ -6861,9 +7615,15 @@
       <c r="B220" s="4" t="s">
         <v>541</v>
       </c>
-      <c r="C220" s="9"/>
-      <c r="D220" s="4"/>
-      <c r="E220" s="10"/>
+      <c r="C220" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D220" s="4" t="s">
+        <v>753</v>
+      </c>
+      <c r="E220" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F220" s="11" t="s">
         <v>281</v>
       </c>
@@ -6875,9 +7635,15 @@
       <c r="B221" s="4" t="s">
         <v>542</v>
       </c>
-      <c r="C221" s="9"/>
-      <c r="D221" s="4"/>
-      <c r="E221" s="10"/>
+      <c r="C221" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D221" s="4" t="s">
+        <v>754</v>
+      </c>
+      <c r="E221" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F221" s="11" t="s">
         <v>282</v>
       </c>
@@ -6889,9 +7655,15 @@
       <c r="B222" s="4" t="s">
         <v>543</v>
       </c>
-      <c r="C222" s="9"/>
-      <c r="D222" s="4"/>
-      <c r="E222" s="10"/>
+      <c r="C222" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D222" s="4" t="s">
+        <v>755</v>
+      </c>
+      <c r="E222" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F222" s="11" t="s">
         <v>283</v>
       </c>
@@ -6903,9 +7675,15 @@
       <c r="B223" s="4" t="s">
         <v>544</v>
       </c>
-      <c r="C223" s="9"/>
-      <c r="D223" s="4"/>
-      <c r="E223" s="10"/>
+      <c r="C223" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D223" s="4" t="s">
+        <v>756</v>
+      </c>
+      <c r="E223" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F223" s="11" t="s">
         <v>284</v>
       </c>
@@ -6917,9 +7695,15 @@
       <c r="B224" s="4" t="s">
         <v>545</v>
       </c>
-      <c r="C224" s="9"/>
-      <c r="D224" s="4"/>
-      <c r="E224" s="10"/>
+      <c r="C224" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D224" s="4" t="s">
+        <v>757</v>
+      </c>
+      <c r="E224" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F224" s="11" t="s">
         <v>285</v>
       </c>
@@ -6931,9 +7715,15 @@
       <c r="B225" s="4" t="s">
         <v>546</v>
       </c>
-      <c r="C225" s="9"/>
-      <c r="D225" s="4"/>
-      <c r="E225" s="10"/>
+      <c r="C225" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D225" s="4" t="s">
+        <v>758</v>
+      </c>
+      <c r="E225" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F225" s="11" t="s">
         <v>286</v>
       </c>
@@ -6945,9 +7735,15 @@
       <c r="B226" s="4" t="s">
         <v>547</v>
       </c>
-      <c r="C226" s="9"/>
-      <c r="D226" s="4"/>
-      <c r="E226" s="10"/>
+      <c r="C226" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D226" s="4" t="s">
+        <v>759</v>
+      </c>
+      <c r="E226" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F226" s="11" t="s">
         <v>287</v>
       </c>
@@ -6959,9 +7755,15 @@
       <c r="B227" s="4" t="s">
         <v>548</v>
       </c>
-      <c r="C227" s="9"/>
-      <c r="D227" s="4"/>
-      <c r="E227" s="10"/>
+      <c r="C227" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D227" s="4" t="s">
+        <v>760</v>
+      </c>
+      <c r="E227" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F227" s="11" t="s">
         <v>288</v>
       </c>
@@ -6973,9 +7775,15 @@
       <c r="B228" s="4" t="s">
         <v>549</v>
       </c>
-      <c r="C228" s="9"/>
-      <c r="D228" s="4"/>
-      <c r="E228" s="10"/>
+      <c r="C228" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D228" s="4" t="s">
+        <v>761</v>
+      </c>
+      <c r="E228" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F228" s="11" t="s">
         <v>289</v>
       </c>
@@ -6987,9 +7795,15 @@
       <c r="B229" s="4" t="s">
         <v>550</v>
       </c>
-      <c r="C229" s="9"/>
-      <c r="D229" s="4"/>
-      <c r="E229" s="10"/>
+      <c r="C229" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D229" s="4" t="s">
+        <v>762</v>
+      </c>
+      <c r="E229" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F229" s="11" t="s">
         <v>290</v>
       </c>
@@ -7001,9 +7815,15 @@
       <c r="B230" s="4" t="s">
         <v>551</v>
       </c>
-      <c r="C230" s="9"/>
-      <c r="D230" s="4"/>
-      <c r="E230" s="10"/>
+      <c r="C230" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D230" s="4" t="s">
+        <v>763</v>
+      </c>
+      <c r="E230" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F230" s="11" t="s">
         <v>291</v>
       </c>
@@ -7015,9 +7835,15 @@
       <c r="B231" s="4" t="s">
         <v>552</v>
       </c>
-      <c r="C231" s="9"/>
-      <c r="D231" s="4"/>
-      <c r="E231" s="10"/>
+      <c r="C231" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D231" s="4" t="s">
+        <v>764</v>
+      </c>
+      <c r="E231" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F231" s="11" t="s">
         <v>292</v>
       </c>
@@ -7029,9 +7855,15 @@
       <c r="B232" s="4" t="s">
         <v>553</v>
       </c>
-      <c r="C232" s="9"/>
-      <c r="D232" s="4"/>
-      <c r="E232" s="10"/>
+      <c r="C232" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D232" s="4" t="s">
+        <v>765</v>
+      </c>
+      <c r="E232" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F232" s="11" t="s">
         <v>293</v>
       </c>
@@ -7043,9 +7875,15 @@
       <c r="B233" s="4" t="s">
         <v>554</v>
       </c>
-      <c r="C233" s="9"/>
-      <c r="D233" s="4"/>
-      <c r="E233" s="10"/>
+      <c r="C233" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D233" s="4" t="s">
+        <v>766</v>
+      </c>
+      <c r="E233" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F233" s="11" t="s">
         <v>294</v>
       </c>
@@ -7057,9 +7895,15 @@
       <c r="B234" s="4" t="s">
         <v>555</v>
       </c>
-      <c r="C234" s="9"/>
-      <c r="D234" s="4"/>
-      <c r="E234" s="10"/>
+      <c r="C234" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D234" s="4" t="s">
+        <v>767</v>
+      </c>
+      <c r="E234" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F234" s="11" t="s">
         <v>295</v>
       </c>
@@ -7071,9 +7915,15 @@
       <c r="B235" s="4" t="s">
         <v>556</v>
       </c>
-      <c r="C235" s="9"/>
-      <c r="D235" s="4"/>
-      <c r="E235" s="10"/>
+      <c r="C235" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D235" s="4" t="s">
+        <v>768</v>
+      </c>
+      <c r="E235" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F235" s="11" t="s">
         <v>296</v>
       </c>
@@ -7085,9 +7935,15 @@
       <c r="B236" s="4" t="s">
         <v>557</v>
       </c>
-      <c r="C236" s="9"/>
-      <c r="D236" s="4"/>
-      <c r="E236" s="10"/>
+      <c r="C236" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D236" s="4" t="s">
+        <v>769</v>
+      </c>
+      <c r="E236" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F236" s="11" t="s">
         <v>297</v>
       </c>
@@ -7099,9 +7955,15 @@
       <c r="B237" s="4" t="s">
         <v>558</v>
       </c>
-      <c r="C237" s="9"/>
-      <c r="D237" s="4"/>
-      <c r="E237" s="10"/>
+      <c r="C237" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D237" s="4" t="s">
+        <v>770</v>
+      </c>
+      <c r="E237" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F237" s="11" t="s">
         <v>298</v>
       </c>
@@ -7113,9 +7975,15 @@
       <c r="B238" s="4" t="s">
         <v>559</v>
       </c>
-      <c r="C238" s="9"/>
-      <c r="D238" s="4"/>
-      <c r="E238" s="10"/>
+      <c r="C238" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D238" s="4" t="s">
+        <v>771</v>
+      </c>
+      <c r="E238" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F238" s="11" t="s">
         <v>299</v>
       </c>
@@ -7127,9 +7995,15 @@
       <c r="B239" s="4" t="s">
         <v>560</v>
       </c>
-      <c r="C239" s="9"/>
-      <c r="D239" s="4"/>
-      <c r="E239" s="10"/>
+      <c r="C239" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D239" s="4" t="s">
+        <v>772</v>
+      </c>
+      <c r="E239" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F239" s="11" t="s">
         <v>300</v>
       </c>
@@ -7141,9 +8015,15 @@
       <c r="B240" s="4" t="s">
         <v>561</v>
       </c>
-      <c r="C240" s="9"/>
-      <c r="D240" s="4"/>
-      <c r="E240" s="10"/>
+      <c r="C240" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D240" s="4" t="s">
+        <v>773</v>
+      </c>
+      <c r="E240" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F240" s="11" t="s">
         <v>301</v>
       </c>
@@ -7155,9 +8035,15 @@
       <c r="B241" s="4" t="s">
         <v>562</v>
       </c>
-      <c r="C241" s="9"/>
-      <c r="D241" s="4"/>
-      <c r="E241" s="10"/>
+      <c r="C241" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D241" s="4" t="s">
+        <v>774</v>
+      </c>
+      <c r="E241" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F241" s="11" t="s">
         <v>302</v>
       </c>
@@ -7169,9 +8055,15 @@
       <c r="B242" s="4" t="s">
         <v>563</v>
       </c>
-      <c r="C242" s="9"/>
-      <c r="D242" s="4"/>
-      <c r="E242" s="10"/>
+      <c r="C242" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D242" s="4" t="s">
+        <v>775</v>
+      </c>
+      <c r="E242" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F242" s="11" t="s">
         <v>303</v>
       </c>
@@ -7183,9 +8075,15 @@
       <c r="B243" s="4" t="s">
         <v>564</v>
       </c>
-      <c r="C243" s="9"/>
-      <c r="D243" s="4"/>
-      <c r="E243" s="10"/>
+      <c r="C243" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D243" s="4" t="s">
+        <v>776</v>
+      </c>
+      <c r="E243" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F243" s="11" t="s">
         <v>304</v>
       </c>
@@ -7197,9 +8095,15 @@
       <c r="B244" s="4" t="s">
         <v>565</v>
       </c>
-      <c r="C244" s="9"/>
-      <c r="D244" s="4"/>
-      <c r="E244" s="10"/>
+      <c r="C244" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D244" s="4" t="s">
+        <v>777</v>
+      </c>
+      <c r="E244" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F244" s="11" t="s">
         <v>305</v>
       </c>
@@ -7211,9 +8115,15 @@
       <c r="B245" s="4" t="s">
         <v>566</v>
       </c>
-      <c r="C245" s="9"/>
-      <c r="D245" s="4"/>
-      <c r="E245" s="10"/>
+      <c r="C245" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D245" s="4" t="s">
+        <v>778</v>
+      </c>
+      <c r="E245" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F245" s="11" t="s">
         <v>306</v>
       </c>
@@ -7225,9 +8135,15 @@
       <c r="B246" s="4" t="s">
         <v>567</v>
       </c>
-      <c r="C246" s="9"/>
-      <c r="D246" s="4"/>
-      <c r="E246" s="10"/>
+      <c r="C246" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D246" s="4" t="s">
+        <v>779</v>
+      </c>
+      <c r="E246" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F246" s="11" t="s">
         <v>307</v>
       </c>
@@ -7239,9 +8155,15 @@
       <c r="B247" s="4" t="s">
         <v>568</v>
       </c>
-      <c r="C247" s="9"/>
-      <c r="D247" s="4"/>
-      <c r="E247" s="10"/>
+      <c r="C247" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D247" s="4" t="s">
+        <v>780</v>
+      </c>
+      <c r="E247" s="10" t="s">
+        <v>660</v>
+      </c>
       <c r="F247" s="11" t="s">
         <v>308</v>
       </c>
@@ -7653,9 +8575,15 @@
       <c r="B268" s="4" t="s">
         <v>589</v>
       </c>
-      <c r="C268" s="9"/>
-      <c r="D268" s="4"/>
-      <c r="E268" s="10"/>
+      <c r="C268" s="9" t="s">
+        <v>782</v>
+      </c>
+      <c r="D268" s="4" t="s">
+        <v>783</v>
+      </c>
+      <c r="E268" s="10" t="s">
+        <v>781</v>
+      </c>
       <c r="F268" s="11" t="s">
         <v>309</v>
       </c>
@@ -7667,9 +8595,15 @@
       <c r="B269" s="4" t="s">
         <v>590</v>
       </c>
-      <c r="C269" s="9"/>
-      <c r="D269" s="4"/>
-      <c r="E269" s="10"/>
+      <c r="C269" s="9" t="s">
+        <v>782</v>
+      </c>
+      <c r="D269" s="4" t="s">
+        <v>784</v>
+      </c>
+      <c r="E269" s="10" t="s">
+        <v>781</v>
+      </c>
       <c r="F269" s="11" t="s">
         <v>310</v>
       </c>
@@ -7681,9 +8615,15 @@
       <c r="B270" s="4" t="s">
         <v>591</v>
       </c>
-      <c r="C270" s="9"/>
-      <c r="D270" s="4"/>
-      <c r="E270" s="10"/>
+      <c r="C270" s="9" t="s">
+        <v>782</v>
+      </c>
+      <c r="D270" s="4" t="s">
+        <v>785</v>
+      </c>
+      <c r="E270" s="10" t="s">
+        <v>781</v>
+      </c>
       <c r="F270" s="11" t="s">
         <v>311</v>
       </c>
@@ -7695,11 +8635,17 @@
       <c r="B271" s="4" t="s">
         <v>592</v>
       </c>
-      <c r="C271" s="9"/>
-      <c r="D271" s="4"/>
-      <c r="E271" s="10"/>
+      <c r="C271" s="9" t="s">
+        <v>782</v>
+      </c>
+      <c r="D271" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="E271" s="10" t="s">
+        <v>781</v>
+      </c>
       <c r="F271" s="11" t="s">
-        <v>311</v>
+        <v>787</v>
       </c>
     </row>
     <row r="272" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -7709,9 +8655,15 @@
       <c r="B272" s="4" t="s">
         <v>593</v>
       </c>
-      <c r="C272" s="9"/>
-      <c r="D272" s="4"/>
-      <c r="E272" s="10"/>
+      <c r="C272" s="9" t="s">
+        <v>782</v>
+      </c>
+      <c r="D272" s="4" t="s">
+        <v>789</v>
+      </c>
+      <c r="E272" s="10" t="s">
+        <v>781</v>
+      </c>
       <c r="F272" s="11" t="s">
         <v>312</v>
       </c>
@@ -7723,9 +8675,15 @@
       <c r="B273" s="4" t="s">
         <v>594</v>
       </c>
-      <c r="C273" s="9"/>
-      <c r="D273" s="4"/>
-      <c r="E273" s="10"/>
+      <c r="C273" s="9" t="s">
+        <v>782</v>
+      </c>
+      <c r="D273" s="4" t="s">
+        <v>790</v>
+      </c>
+      <c r="E273" s="10" t="s">
+        <v>781</v>
+      </c>
       <c r="F273" s="11" t="s">
         <v>313</v>
       </c>
@@ -7737,9 +8695,15 @@
       <c r="B274" s="4" t="s">
         <v>595</v>
       </c>
-      <c r="C274" s="9"/>
-      <c r="D274" s="4"/>
-      <c r="E274" s="10"/>
+      <c r="C274" s="9" t="s">
+        <v>782</v>
+      </c>
+      <c r="D274" s="4" t="s">
+        <v>791</v>
+      </c>
+      <c r="E274" s="10" t="s">
+        <v>781</v>
+      </c>
       <c r="F274" s="11" t="s">
         <v>314</v>
       </c>
@@ -7751,9 +8715,15 @@
       <c r="B275" s="4" t="s">
         <v>596</v>
       </c>
-      <c r="C275" s="9"/>
-      <c r="D275" s="4"/>
-      <c r="E275" s="10"/>
+      <c r="C275" s="9" t="s">
+        <v>782</v>
+      </c>
+      <c r="D275" s="4" t="s">
+        <v>792</v>
+      </c>
+      <c r="E275" s="10" t="s">
+        <v>781</v>
+      </c>
       <c r="F275" s="11" t="s">
         <v>315</v>
       </c>
@@ -7765,9 +8735,15 @@
       <c r="B276" s="4" t="s">
         <v>597</v>
       </c>
-      <c r="C276" s="9"/>
-      <c r="D276" s="4"/>
-      <c r="E276" s="10"/>
+      <c r="C276" s="9" t="s">
+        <v>782</v>
+      </c>
+      <c r="D276" s="4" t="s">
+        <v>793</v>
+      </c>
+      <c r="E276" s="10" t="s">
+        <v>781</v>
+      </c>
       <c r="F276" s="11" t="s">
         <v>316</v>
       </c>
@@ -7779,9 +8755,15 @@
       <c r="B277" s="4" t="s">
         <v>598</v>
       </c>
-      <c r="C277" s="9"/>
-      <c r="D277" s="4"/>
-      <c r="E277" s="10"/>
+      <c r="C277" s="9" t="s">
+        <v>782</v>
+      </c>
+      <c r="D277" s="4" t="s">
+        <v>794</v>
+      </c>
+      <c r="E277" s="10" t="s">
+        <v>781</v>
+      </c>
       <c r="F277" s="11" t="s">
         <v>317</v>
       </c>
@@ -7793,9 +8775,15 @@
       <c r="B278" s="4" t="s">
         <v>599</v>
       </c>
-      <c r="C278" s="9"/>
-      <c r="D278" s="4"/>
-      <c r="E278" s="10"/>
+      <c r="C278" s="9" t="s">
+        <v>782</v>
+      </c>
+      <c r="D278" s="4" t="s">
+        <v>795</v>
+      </c>
+      <c r="E278" s="10" t="s">
+        <v>781</v>
+      </c>
       <c r="F278" s="11" t="s">
         <v>318</v>
       </c>
@@ -7807,11 +8795,17 @@
       <c r="B279" s="4" t="s">
         <v>600</v>
       </c>
-      <c r="C279" s="9"/>
-      <c r="D279" s="4"/>
-      <c r="E279" s="10"/>
+      <c r="C279" s="9" t="s">
+        <v>782</v>
+      </c>
+      <c r="D279" s="4" t="s">
+        <v>796</v>
+      </c>
+      <c r="E279" s="10" t="s">
+        <v>781</v>
+      </c>
       <c r="F279" s="11" t="s">
-        <v>318</v>
+        <v>786</v>
       </c>
     </row>
     <row r="280" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -7821,9 +8815,15 @@
       <c r="B280" s="4" t="s">
         <v>601</v>
       </c>
-      <c r="C280" s="9"/>
-      <c r="D280" s="4"/>
-      <c r="E280" s="10"/>
+      <c r="C280" s="9" t="s">
+        <v>782</v>
+      </c>
+      <c r="D280" s="4" t="s">
+        <v>797</v>
+      </c>
+      <c r="E280" s="10" t="s">
+        <v>781</v>
+      </c>
       <c r="F280" s="11" t="s">
         <v>319</v>
       </c>
@@ -7835,9 +8835,15 @@
       <c r="B281" s="4" t="s">
         <v>602</v>
       </c>
-      <c r="C281" s="9"/>
-      <c r="D281" s="4"/>
-      <c r="E281" s="10"/>
+      <c r="C281" s="9" t="s">
+        <v>782</v>
+      </c>
+      <c r="D281" s="4" t="s">
+        <v>798</v>
+      </c>
+      <c r="E281" s="10" t="s">
+        <v>781</v>
+      </c>
       <c r="F281" s="11" t="s">
         <v>320</v>
       </c>
@@ -7849,9 +8855,15 @@
       <c r="B282" s="4" t="s">
         <v>603</v>
       </c>
-      <c r="C282" s="9"/>
-      <c r="D282" s="4"/>
-      <c r="E282" s="10"/>
+      <c r="C282" s="9" t="s">
+        <v>782</v>
+      </c>
+      <c r="D282" s="4" t="s">
+        <v>799</v>
+      </c>
+      <c r="E282" s="10" t="s">
+        <v>781</v>
+      </c>
       <c r="F282" s="11" t="s">
         <v>321</v>
       </c>
@@ -7863,9 +8875,15 @@
       <c r="B283" s="4" t="s">
         <v>604</v>
       </c>
-      <c r="C283" s="9"/>
-      <c r="D283" s="4"/>
-      <c r="E283" s="10"/>
+      <c r="C283" s="9" t="s">
+        <v>782</v>
+      </c>
+      <c r="D283" s="4" t="s">
+        <v>800</v>
+      </c>
+      <c r="E283" s="10" t="s">
+        <v>781</v>
+      </c>
       <c r="F283" s="11" t="s">
         <v>322</v>
       </c>
@@ -7877,9 +8895,15 @@
       <c r="B284" s="4" t="s">
         <v>605</v>
       </c>
-      <c r="C284" s="8"/>
-      <c r="D284" s="5"/>
-      <c r="E284" s="6"/>
+      <c r="C284" s="9" t="s">
+        <v>782</v>
+      </c>
+      <c r="D284" s="4" t="s">
+        <v>800</v>
+      </c>
+      <c r="E284" s="10" t="s">
+        <v>781</v>
+      </c>
       <c r="F284" s="12" t="s">
         <v>322</v>
       </c>
@@ -7893,4 +8917,727 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25F8B4CA-AD1D-4E6B-BDB6-617CA9B7EFFA}">
+  <dimension ref="D3:F61"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:F61"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D3" s="11" t="s">
+        <v>676</v>
+      </c>
+      <c r="E3" t="s">
+        <v>720</v>
+      </c>
+      <c r="F3" t="str">
+        <f>D3&amp;","&amp;E3</f>
+        <v>Japanese,YES,YES,K,DESCR</v>
+      </c>
+    </row>
+    <row r="4" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D4" s="13" t="s">
+        <v>677</v>
+      </c>
+      <c r="E4" t="s">
+        <v>720</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" ref="F4:F61" si="0">D4&amp;","&amp;E4</f>
+        <v>Japanese,YES,YES,MLN,DESCR</v>
+      </c>
+    </row>
+    <row r="5" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D5" s="11" t="s">
+        <v>679</v>
+      </c>
+      <c r="E5" t="s">
+        <v>720</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>Japanese,YES,YES,BLN,DESCR</v>
+      </c>
+    </row>
+    <row r="6" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D6" s="13" t="s">
+        <v>678</v>
+      </c>
+      <c r="E6" t="s">
+        <v>720</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>Japanese,YES,YES,TRLN,DESCR</v>
+      </c>
+    </row>
+    <row r="7" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D7" s="11" t="s">
+        <v>680</v>
+      </c>
+      <c r="E7" t="s">
+        <v>720</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>English,YES,YES,SINGLE,DESCR</v>
+      </c>
+    </row>
+    <row r="8" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D8" s="13" t="s">
+        <v>681</v>
+      </c>
+      <c r="E8" t="s">
+        <v>720</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>English,YES,YES,K,DESCR</v>
+      </c>
+    </row>
+    <row r="9" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D9" s="11" t="s">
+        <v>682</v>
+      </c>
+      <c r="E9" t="s">
+        <v>720</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>English,YES,YES,MLN,DESCR</v>
+      </c>
+    </row>
+    <row r="10" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D10" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="E10" t="s">
+        <v>720</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>English,YES,YES,BLN,DESCR</v>
+      </c>
+    </row>
+    <row r="11" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D11" s="11" t="s">
+        <v>684</v>
+      </c>
+      <c r="E11" t="s">
+        <v>720</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>English,YES,YES,TRLN,DESCR</v>
+      </c>
+    </row>
+    <row r="12" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D12" s="13" t="s">
+        <v>685</v>
+      </c>
+      <c r="E12" t="s">
+        <v>720</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>French,YES,YES,SINGLE,DESCR</v>
+      </c>
+    </row>
+    <row r="13" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D13" s="11" t="s">
+        <v>686</v>
+      </c>
+      <c r="E13" t="s">
+        <v>720</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>French,YES,YES,K,DESCR</v>
+      </c>
+    </row>
+    <row r="14" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D14" s="13" t="s">
+        <v>687</v>
+      </c>
+      <c r="E14" t="s">
+        <v>720</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>French,YES,YES,MLN,DESCR</v>
+      </c>
+    </row>
+    <row r="15" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D15" s="11" t="s">
+        <v>688</v>
+      </c>
+      <c r="E15" t="s">
+        <v>720</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>French,YES,YES,BLN,DESCR</v>
+      </c>
+    </row>
+    <row r="16" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D16" s="13" t="s">
+        <v>689</v>
+      </c>
+      <c r="E16" t="s">
+        <v>720</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
+        <v>French,YES,YES,TRLN,DESCR</v>
+      </c>
+    </row>
+    <row r="17" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D17" s="11" t="s">
+        <v>661</v>
+      </c>
+      <c r="E17" t="s">
+        <v>720</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="0"/>
+        <v>Japanese,NO,NO,SINGLE,DESCR</v>
+      </c>
+    </row>
+    <row r="18" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D18" s="13" t="s">
+        <v>662</v>
+      </c>
+      <c r="E18" t="s">
+        <v>720</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="0"/>
+        <v>Japanese,NO,NO,K,DESCR</v>
+      </c>
+    </row>
+    <row r="19" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D19" s="11" t="s">
+        <v>663</v>
+      </c>
+      <c r="E19" t="s">
+        <v>720</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="0"/>
+        <v>Japanese,NO,NO,MLN,DESCR</v>
+      </c>
+    </row>
+    <row r="20" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D20" s="13" t="s">
+        <v>664</v>
+      </c>
+      <c r="E20" t="s">
+        <v>720</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="0"/>
+        <v>Japanese,NO,NO,BLN,DESCR</v>
+      </c>
+    </row>
+    <row r="21" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D21" s="11" t="s">
+        <v>665</v>
+      </c>
+      <c r="E21" t="s">
+        <v>720</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="0"/>
+        <v>Japanese,NO,NO,TRLN,DESCR</v>
+      </c>
+    </row>
+    <row r="22" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D22" s="13" t="s">
+        <v>666</v>
+      </c>
+      <c r="E22" t="s">
+        <v>720</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="0"/>
+        <v>English,NO,NO,SINGLE,DESCR</v>
+      </c>
+    </row>
+    <row r="23" spans="4:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D23" s="11" t="s">
+        <v>667</v>
+      </c>
+      <c r="E23" t="s">
+        <v>720</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="0"/>
+        <v>English,NO,NO,K,DESCR</v>
+      </c>
+    </row>
+    <row r="24" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D24" s="13" t="s">
+        <v>668</v>
+      </c>
+      <c r="E24" t="s">
+        <v>720</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="0"/>
+        <v>English,NO,NO,MLN,DESCR</v>
+      </c>
+    </row>
+    <row r="25" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D25" s="11" t="s">
+        <v>669</v>
+      </c>
+      <c r="E25" t="s">
+        <v>720</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="0"/>
+        <v>English,NO,NO,BLN,DESCR</v>
+      </c>
+    </row>
+    <row r="26" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D26" s="13" t="s">
+        <v>670</v>
+      </c>
+      <c r="E26" t="s">
+        <v>720</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="0"/>
+        <v>English,NO,NO,TRLN,DESCR</v>
+      </c>
+    </row>
+    <row r="27" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D27" s="11" t="s">
+        <v>671</v>
+      </c>
+      <c r="E27" t="s">
+        <v>720</v>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" si="0"/>
+        <v>French,NO,NO,SINGLE,DESCR</v>
+      </c>
+    </row>
+    <row r="28" spans="4:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D28" s="13" t="s">
+        <v>672</v>
+      </c>
+      <c r="E28" t="s">
+        <v>720</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" si="0"/>
+        <v>French,NO,NO,K,DESCR</v>
+      </c>
+    </row>
+    <row r="29" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D29" s="11" t="s">
+        <v>673</v>
+      </c>
+      <c r="E29" t="s">
+        <v>720</v>
+      </c>
+      <c r="F29" t="str">
+        <f t="shared" si="0"/>
+        <v>French,NO,NO,MLN,DESCR</v>
+      </c>
+    </row>
+    <row r="30" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D30" s="13" t="s">
+        <v>674</v>
+      </c>
+      <c r="E30" t="s">
+        <v>720</v>
+      </c>
+      <c r="F30" t="str">
+        <f t="shared" si="0"/>
+        <v>French,NO,NO,BLN,DESCR</v>
+      </c>
+    </row>
+    <row r="31" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D31" s="11" t="s">
+        <v>675</v>
+      </c>
+      <c r="E31" t="s">
+        <v>720</v>
+      </c>
+      <c r="F31" t="str">
+        <f t="shared" si="0"/>
+        <v>French,NO,NO,TRLN,DESCR</v>
+      </c>
+    </row>
+    <row r="32" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D32" s="13" t="s">
+        <v>690</v>
+      </c>
+      <c r="E32" t="s">
+        <v>720</v>
+      </c>
+      <c r="F32" t="str">
+        <f t="shared" si="0"/>
+        <v>Japanese,YES,NO,SINGLE,DESCR</v>
+      </c>
+    </row>
+    <row r="33" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D33" s="11" t="s">
+        <v>691</v>
+      </c>
+      <c r="E33" t="s">
+        <v>720</v>
+      </c>
+      <c r="F33" t="str">
+        <f t="shared" si="0"/>
+        <v>Japanese,YES,NO,K,DESCR</v>
+      </c>
+    </row>
+    <row r="34" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D34" s="13" t="s">
+        <v>692</v>
+      </c>
+      <c r="E34" t="s">
+        <v>720</v>
+      </c>
+      <c r="F34" t="str">
+        <f t="shared" si="0"/>
+        <v>Japanese,YES,NO,MLN,DESCR</v>
+      </c>
+    </row>
+    <row r="35" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D35" s="11" t="s">
+        <v>693</v>
+      </c>
+      <c r="E35" t="s">
+        <v>720</v>
+      </c>
+      <c r="F35" t="str">
+        <f t="shared" si="0"/>
+        <v>Japanese,YES,NO,BLN,DESCR</v>
+      </c>
+    </row>
+    <row r="36" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D36" s="13" t="s">
+        <v>694</v>
+      </c>
+      <c r="E36" t="s">
+        <v>720</v>
+      </c>
+      <c r="F36" t="str">
+        <f t="shared" si="0"/>
+        <v>Japanese,YES,NO,TRLN,DESCR</v>
+      </c>
+    </row>
+    <row r="37" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D37" s="11" t="s">
+        <v>695</v>
+      </c>
+      <c r="E37" t="s">
+        <v>720</v>
+      </c>
+      <c r="F37" t="str">
+        <f t="shared" si="0"/>
+        <v>English,YES,NO,SINGLE,DESCR</v>
+      </c>
+    </row>
+    <row r="38" spans="4:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D38" s="13" t="s">
+        <v>696</v>
+      </c>
+      <c r="E38" t="s">
+        <v>720</v>
+      </c>
+      <c r="F38" t="str">
+        <f t="shared" si="0"/>
+        <v>English,YES,NO,K,DESCR</v>
+      </c>
+    </row>
+    <row r="39" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D39" s="11" t="s">
+        <v>697</v>
+      </c>
+      <c r="E39" t="s">
+        <v>720</v>
+      </c>
+      <c r="F39" t="str">
+        <f t="shared" si="0"/>
+        <v>English,YES,NO,MLN,DESCR</v>
+      </c>
+    </row>
+    <row r="40" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D40" s="13" t="s">
+        <v>698</v>
+      </c>
+      <c r="E40" t="s">
+        <v>720</v>
+      </c>
+      <c r="F40" t="str">
+        <f t="shared" si="0"/>
+        <v>English,YES,NO,BLN,DESCR</v>
+      </c>
+    </row>
+    <row r="41" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D41" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="E41" t="s">
+        <v>720</v>
+      </c>
+      <c r="F41" t="str">
+        <f t="shared" si="0"/>
+        <v>English,YES,NO,TRLN,DESCR</v>
+      </c>
+    </row>
+    <row r="42" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D42" s="13" t="s">
+        <v>700</v>
+      </c>
+      <c r="E42" t="s">
+        <v>720</v>
+      </c>
+      <c r="F42" t="str">
+        <f t="shared" si="0"/>
+        <v>French,YES,NO,SINGLE,DESCR</v>
+      </c>
+    </row>
+    <row r="43" spans="4:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D43" s="11" t="s">
+        <v>701</v>
+      </c>
+      <c r="E43" t="s">
+        <v>720</v>
+      </c>
+      <c r="F43" t="str">
+        <f t="shared" si="0"/>
+        <v>French,YES,NO,K,DESCR</v>
+      </c>
+    </row>
+    <row r="44" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D44" s="13" t="s">
+        <v>702</v>
+      </c>
+      <c r="E44" t="s">
+        <v>720</v>
+      </c>
+      <c r="F44" t="str">
+        <f t="shared" si="0"/>
+        <v>French,YES,NO,MLN,DESCR</v>
+      </c>
+    </row>
+    <row r="45" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D45" s="11" t="s">
+        <v>703</v>
+      </c>
+      <c r="E45" t="s">
+        <v>720</v>
+      </c>
+      <c r="F45" t="str">
+        <f t="shared" si="0"/>
+        <v>French,YES,NO,BLN,DESCR</v>
+      </c>
+    </row>
+    <row r="46" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D46" s="13" t="s">
+        <v>704</v>
+      </c>
+      <c r="E46" t="s">
+        <v>720</v>
+      </c>
+      <c r="F46" t="str">
+        <f t="shared" si="0"/>
+        <v>French,YES,NO,TRLN,DESCR</v>
+      </c>
+    </row>
+    <row r="47" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D47" s="11" t="s">
+        <v>705</v>
+      </c>
+      <c r="E47" t="s">
+        <v>720</v>
+      </c>
+      <c r="F47" t="str">
+        <f t="shared" si="0"/>
+        <v>Japanese,NO,YES,SINGLE,DESCR</v>
+      </c>
+    </row>
+    <row r="48" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D48" s="13" t="s">
+        <v>706</v>
+      </c>
+      <c r="E48" t="s">
+        <v>720</v>
+      </c>
+      <c r="F48" t="str">
+        <f t="shared" si="0"/>
+        <v>Japanese,NO,YES,K,DESCR</v>
+      </c>
+    </row>
+    <row r="49" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D49" s="11" t="s">
+        <v>707</v>
+      </c>
+      <c r="E49" t="s">
+        <v>720</v>
+      </c>
+      <c r="F49" t="str">
+        <f t="shared" si="0"/>
+        <v>Japanese,NO,YES,MLN,DESCR</v>
+      </c>
+    </row>
+    <row r="50" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D50" s="13" t="s">
+        <v>708</v>
+      </c>
+      <c r="E50" t="s">
+        <v>720</v>
+      </c>
+      <c r="F50" t="str">
+        <f t="shared" si="0"/>
+        <v>Japanese,NO,YES,BLN,DESCR</v>
+      </c>
+    </row>
+    <row r="51" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D51" s="11" t="s">
+        <v>709</v>
+      </c>
+      <c r="E51" t="s">
+        <v>720</v>
+      </c>
+      <c r="F51" t="str">
+        <f t="shared" si="0"/>
+        <v>Japanese,NO,YES,TRLN,DESCR</v>
+      </c>
+    </row>
+    <row r="52" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D52" s="13" t="s">
+        <v>710</v>
+      </c>
+      <c r="E52" t="s">
+        <v>720</v>
+      </c>
+      <c r="F52" t="str">
+        <f t="shared" si="0"/>
+        <v>English,NO,YES,SINGLE,DESCR</v>
+      </c>
+    </row>
+    <row r="53" spans="4:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D53" s="11" t="s">
+        <v>711</v>
+      </c>
+      <c r="E53" t="s">
+        <v>720</v>
+      </c>
+      <c r="F53" t="str">
+        <f t="shared" si="0"/>
+        <v>English,NO,YES,K,DESCR</v>
+      </c>
+    </row>
+    <row r="54" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D54" s="13" t="s">
+        <v>712</v>
+      </c>
+      <c r="E54" t="s">
+        <v>720</v>
+      </c>
+      <c r="F54" t="str">
+        <f t="shared" si="0"/>
+        <v>English,NO,YES,MLN,DESCR</v>
+      </c>
+    </row>
+    <row r="55" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D55" s="11" t="s">
+        <v>713</v>
+      </c>
+      <c r="E55" t="s">
+        <v>720</v>
+      </c>
+      <c r="F55" t="str">
+        <f t="shared" si="0"/>
+        <v>English,NO,YES,BLN,DESCR</v>
+      </c>
+    </row>
+    <row r="56" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D56" s="13" t="s">
+        <v>714</v>
+      </c>
+      <c r="E56" t="s">
+        <v>720</v>
+      </c>
+      <c r="F56" t="str">
+        <f t="shared" si="0"/>
+        <v>English,NO,YES,TRLN,DESCR</v>
+      </c>
+    </row>
+    <row r="57" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D57" s="11" t="s">
+        <v>715</v>
+      </c>
+      <c r="E57" t="s">
+        <v>720</v>
+      </c>
+      <c r="F57" t="str">
+        <f t="shared" si="0"/>
+        <v>French,NO,YES,SINGLE,DESCR</v>
+      </c>
+    </row>
+    <row r="58" spans="4:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D58" s="13" t="s">
+        <v>716</v>
+      </c>
+      <c r="E58" t="s">
+        <v>720</v>
+      </c>
+      <c r="F58" t="str">
+        <f t="shared" si="0"/>
+        <v>French,NO,YES,K,DESCR</v>
+      </c>
+    </row>
+    <row r="59" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D59" s="11" t="s">
+        <v>717</v>
+      </c>
+      <c r="E59" t="s">
+        <v>720</v>
+      </c>
+      <c r="F59" t="str">
+        <f t="shared" si="0"/>
+        <v>French,NO,YES,MLN,DESCR</v>
+      </c>
+    </row>
+    <row r="60" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D60" s="13" t="s">
+        <v>718</v>
+      </c>
+      <c r="E60" t="s">
+        <v>720</v>
+      </c>
+      <c r="F60" t="str">
+        <f t="shared" si="0"/>
+        <v>French,NO,YES,BLN,DESCR</v>
+      </c>
+    </row>
+    <row r="61" spans="4:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D61" s="11" t="s">
+        <v>719</v>
+      </c>
+      <c r="E61" t="s">
+        <v>720</v>
+      </c>
+      <c r="F61" t="str">
+        <f t="shared" si="0"/>
+        <v>French,NO,YES,TRLN,DESCR</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>